<commit_message>
73600-working as per the spec but using a seperate body template
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Service/Reports/Templates/SummaryOfFM35FundingBody.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Service/Reports/Templates/SummaryOfFM35FundingBody.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gayatri\source\repos\DC-ILR-1819-ReportService\src\ESFA.DC.ILR.ReportService.Service\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF32393-E9DD-49DA-A5DE-2DA7951CC4D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470BDF02-92B1-4E2E-9A98-498AE0A5C6BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="9240" windowHeight="15600" xr2:uid="{F859CCD3-14F9-4B4C-B07D-F3D99CEDF1D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F859CCD3-14F9-4B4C-B07D-F3D99CEDF1D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Funding Line Type</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Period</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Totals</t>
   </si>
   <si>
@@ -65,43 +62,31 @@
     <t>Total (£)</t>
   </si>
   <si>
-    <t>&amp;=GroupedModels[1].OnProgramme</t>
-  </si>
-  <si>
-    <t>&amp;=GroupedModels[2].OnProgramme</t>
-  </si>
-  <si>
-    <t>&amp;=GroupedModels[3].OnProgramme</t>
-  </si>
-  <si>
-    <t>&amp;=GroupedModels[4].OnProgramme</t>
-  </si>
-  <si>
-    <t>&amp;=GroupedModels[5].OnProgramme</t>
-  </si>
-  <si>
-    <t>&amp;=GroupedModels[6].OnProgramme</t>
-  </si>
-  <si>
-    <t>&amp;=GroupedModels[7].OnProgramme</t>
-  </si>
-  <si>
-    <t>&amp;=GroupedModels[8].OnProgramme</t>
-  </si>
-  <si>
-    <t>&amp;=GroupedModels[9].OnProgramme</t>
-  </si>
-  <si>
-    <t>&amp;=GroupedModels[10].OnProgramme</t>
-  </si>
-  <si>
-    <t>&amp;=GroupedModels[11].OnProgramme</t>
-  </si>
-  <si>
-    <t>&amp;=$FundLine</t>
-  </si>
-  <si>
-    <t>&amp;=$GroupedModels[0].OnProgramme</t>
+    <t>&amp;=GroupedModels.OnProgramme</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.Period</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.Balancing</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.JobOutcomeAchievement</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.TotalAchievement</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.AimAchievement</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.LearningSupport</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.Total</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.FundingLineType</t>
   </si>
 </sst>
 </file>
@@ -490,17 +475,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC44AA6-0890-4B92-BC11-BE5F4D3260BF}">
-  <dimension ref="A1:I14"/>
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="9" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="3" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
@@ -511,246 +499,89 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="34.5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>11</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1">
-        <v>12</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="3">
-        <f>SUM(C2:C13)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:I3" si="0">SUBTOTAL(9,C2:C2)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>